<commit_message>
Jsonui: Task list adjusted
Change-Id: I3c52e7d6fc6d0fca70098f3e35e96b494a955492
</commit_message>
<xml_diff>
--- a/org.eclipse.scout.rt.ui.html/org.eclipse.scout.rt.ui.json/docs/project_mgmt/html_ui_tasks.xlsx
+++ b/org.eclipse.scout.rt.ui.html/org.eclipse.scout.rt.ui.json/docs/project_mgmt/html_ui_tasks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="181">
   <si>
     <t>Java Backend</t>
   </si>
@@ -267,9 +267,6 @@
     <t>42 loc</t>
   </si>
   <si>
-    <t>329 loc</t>
-  </si>
-  <si>
     <t>369 loc</t>
   </si>
   <si>
@@ -422,9 +419,6 @@
     <t>- Wrappen des Html-Guis
 - Schnittstelle von Javascript nach Windows
 - Einbettung von Windows-Komponenten?</t>
-  </si>
-  <si>
-    <t>- HTML 5 Feature</t>
   </si>
   <si>
     <t>- ActivityMap (Planner)</t>
@@ -448,16 +442,10 @@
 - Lasttests via Jmeter</t>
   </si>
   <si>
-    <t>Ausbau waitfor -&gt; Vereinfachung Request-Abarbeitung, weniger Threads, Voraussetzung für zuverlässige Last-Tests und DynaTrace</t>
-  </si>
-  <si>
     <t xml:space="preserve">Optimierung ClientSyncJob / WaitFor </t>
   </si>
   <si>
     <t>Rechtschreibeprüfung im Javascript</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Verlagerung von gui-code aus model (scout.client) nach javascript</t>
@@ -524,13 +512,6 @@
     <t>Resourcen Registrierung</t>
   </si>
   <si>
-    <t>Portlet-Support</t>
-  </si>
-  <si>
-    <t>- icons, ev. mit unterschiedlichen Auflösungen für unterschiedliche Geräte (Mobile)
-- File-Downloads (Excel-Export)</t>
-  </si>
-  <si>
     <t>Locale-Handling</t>
   </si>
   <si>
@@ -546,6 +527,76 @@
 - Projekt-Struktur (Files)
 - Erzeugung der JS-und CSS-Files aus den einzelnen kleinen Dateien inkl. Komprimierung (ein/ausschaltbar für development) (ev. LessCSS, verwenden wir für die RapCss, siehe Projekt org.eclipse.scout.rt.ui.rap.theme.rayo.builder)
 - Ev. Evaluierung Tauglichkeit von Modernizer, Twitter Bootstrap und terrifically.org</t>
+  </si>
+  <si>
+    <t>Connection-Failure-Handling</t>
+  </si>
+  <si>
+    <t>- MessageBox Verbindungsverlust
+- Auto-Retry, ev. mit Gui-Anzeige à la Gmail
+- Idempotenz garantieren (letzte Antwort speichern, Request-Nr hochzählen)
+- Eventuell nicht alles nötig, wenn Web-Sockets verwendet wird</t>
+  </si>
+  <si>
+    <t>- Applikations-Icons (crm.client)
+-  ev. mit unterschiedlichen Auflösungen für unterschiedliche Geräte (Mobile)
+- Icons als svg (wof?)
+- File-Downloads (Excel-Export)</t>
+  </si>
+  <si>
+    <t>Ausbau waitfor -&gt; Vereinfachung Request-Abarbeitung, weniger Threads, Voraussetzung für zuverlässige Last-Tests und DynaTrace
+-&gt; waitfor Kann nicht ausgebaut werden, Task beschränkt sich auf Einbau des neuen ClientJob-Mechanismus</t>
+  </si>
+  <si>
+    <t>- BrowserField</t>
+  </si>
+  <si>
+    <t>329 loc, für editable table, komplett in gui umsetzen</t>
+  </si>
+  <si>
+    <t>Request-Optimierung</t>
+  </si>
+  <si>
+    <t>- Nur an den Server, falls nötig 
+- Prüfung auf method override? Attached Listeners? @gui annotation?</t>
+  </si>
+  <si>
+    <t>- HTML 5 Feature
+- benötigt für Table,Tree,Imagefield, vermutlich gerell für alle Felder ermöglichen</t>
+  </si>
+  <si>
+    <t>- Library evaluieren, einbinden</t>
+  </si>
+  <si>
+    <t>Logical Grid Layout</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Library verwenden?</t>
+  </si>
+  <si>
+    <t>kann ev. tree verwenden</t>
+  </si>
+  <si>
+    <t>Multi Split Layout</t>
+  </si>
+  <si>
+    <t>- Anordnung der Forms auf dem Desktop, falls Forms verwendet werden</t>
+  </si>
+  <si>
+    <t>Pages, Outlines, Tabelle, Chart,Graph,Map,Organize</t>
+  </si>
+  <si>
+    <t>Scrolling</t>
+  </si>
+  <si>
+    <t>- Scrolling in Elementen
+- Scrolling on Touch-Devices</t>
+  </si>
+  <si>
+    <t>Client-Seitiger Excel Export</t>
   </si>
 </sst>
 </file>
@@ -962,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K150"/>
+  <dimension ref="A1:K157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="F149" sqref="F149"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,79 +1070,79 @@
     </row>
     <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="9" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>141</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>156</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1101,958 +1152,966 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="3"/>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10" t="s">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="12" t="s">
-        <v>68</v>
+      <c r="F15" s="8" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>30</v>
+        <v>132</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>31</v>
+        <v>165</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="12" t="s">
-        <v>71</v>
-      </c>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="8">
-        <v>10</v>
-      </c>
+      <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>135</v>
+        <v>34</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="12"/>
+      <c r="F26" s="12" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
+      <c r="D27" s="8">
+        <v>10</v>
+      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>16</v>
+        <v>133</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
-      <c r="F28" s="12" t="s">
-        <v>80</v>
-      </c>
+      <c r="F28" s="12"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="12" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
-      <c r="F34" s="12"/>
+      <c r="F34" s="12" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
-      <c r="F36" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="F36" s="12"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
       <c r="F48" s="12" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="8"/>
       <c r="F49" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
       <c r="F50" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
       <c r="E51" s="8"/>
       <c r="F51" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
       <c r="F52" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
       <c r="F53" s="12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
       <c r="F54" s="12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
-        <v>136</v>
+        <v>42</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
       <c r="E55" s="8"/>
-      <c r="F55" s="12"/>
+      <c r="F55" s="12" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
       <c r="E56" s="8"/>
       <c r="F56" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
-        <v>26</v>
+        <v>134</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
       <c r="E57" s="8"/>
-      <c r="F57" s="12" t="s">
-        <v>107</v>
-      </c>
+      <c r="F57" s="12"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
       <c r="E58" s="8"/>
       <c r="F58" s="12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
       <c r="F59" s="12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="8"/>
       <c r="F60" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
       <c r="E61" s="8"/>
       <c r="F61" s="12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
       <c r="E62" s="8"/>
       <c r="F62" s="12" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
       <c r="E63" s="8"/>
       <c r="F63" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
       <c r="E64" s="8"/>
       <c r="F64" s="12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
-      <c r="D65" s="8">
-        <v>10</v>
-      </c>
+      <c r="D65" s="8"/>
       <c r="E65" s="8"/>
       <c r="F65" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
       <c r="F66" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
+      <c r="D67" s="8">
+        <v>10</v>
+      </c>
       <c r="E67" s="8"/>
       <c r="F67" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
       <c r="E68" s="8"/>
       <c r="F68" s="12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
       <c r="E69" s="8"/>
       <c r="F69" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B72" s="7" t="s">
+      <c r="B74" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C74" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D74" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E72" s="7" t="s">
+      <c r="E74" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F72" s="7" t="s">
+      <c r="F74" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A73" s="12" t="s">
+    <row r="75" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A75" s="12" t="s">
         <v>8</v>
-      </c>
-      <c r="B73" s="8"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
-      <c r="F73" s="9" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A74" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B74" s="8"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="8"/>
-      <c r="F74" s="9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="12" t="s">
-        <v>63</v>
       </c>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
       <c r="E75" s="8"/>
       <c r="F75" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="12" t="s">
-        <v>125</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>123</v>
       </c>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
       <c r="E76" s="8"/>
       <c r="F76" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
-        <v>157</v>
+        <v>63</v>
       </c>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
       <c r="E77" s="8"/>
       <c r="F77" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
       <c r="E78" s="8"/>
       <c r="F78" s="9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
       <c r="E79" s="8"/>
       <c r="F79" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="K79" s="13"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
       <c r="E80" s="8"/>
       <c r="F80" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
       <c r="E81" s="8"/>
       <c r="F81" s="9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A82" s="15" t="s">
-        <v>144</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
       <c r="E82" s="8"/>
       <c r="F82" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="15" t="s">
-        <v>161</v>
+        <v>127</v>
+      </c>
+      <c r="K82" s="13"/>
+    </row>
+    <row r="83" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A83" s="12" t="s">
+        <v>130</v>
       </c>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
       <c r="E83" s="8"/>
-      <c r="F83" s="9"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="2"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="3"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="11" t="s">
-        <v>13</v>
+      <c r="F83" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A85" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="15" t="s">
+        <v>178</v>
       </c>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
       <c r="E86" s="8"/>
-      <c r="F86" s="8"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="11" t="s">
-        <v>134</v>
+      <c r="F86" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="15" t="s">
+        <v>180</v>
       </c>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
       <c r="E87" s="8"/>
-      <c r="F87" s="12"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="11" t="s">
-        <v>30</v>
+      <c r="F87" s="9"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="15" t="s">
+        <v>171</v>
       </c>
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
       <c r="E88" s="8"/>
-      <c r="F88" s="12"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="11" t="s">
-        <v>14</v>
+      <c r="F88" s="9"/>
+    </row>
+    <row r="89" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="15" t="s">
+        <v>175</v>
       </c>
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
       <c r="E89" s="8"/>
-      <c r="F89" s="12"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B90" s="8"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="8"/>
-      <c r="F90" s="12"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="12"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F89" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" s="2"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="3"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
       <c r="E92" s="8"/>
-      <c r="F92" s="12"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F92" s="8"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
-        <v>15</v>
+        <v>132</v>
       </c>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
@@ -2060,9 +2119,9 @@
       <c r="E93" s="8"/>
       <c r="F93" s="12"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
@@ -2070,9 +2129,9 @@
       <c r="E94" s="8"/>
       <c r="F94" s="12"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
-        <v>52</v>
+        <v>165</v>
       </c>
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
@@ -2080,9 +2139,9 @@
       <c r="E95" s="8"/>
       <c r="F95" s="12"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
@@ -2092,19 +2151,17 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
-      <c r="D97" s="8">
-        <v>10</v>
-      </c>
+      <c r="D97" s="8"/>
       <c r="E97" s="8"/>
       <c r="F97" s="12"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>137</v>
+        <v>32</v>
       </c>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
@@ -2114,7 +2171,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
@@ -2124,7 +2181,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
@@ -2134,17 +2191,19 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
       <c r="E101" s="8"/>
-      <c r="F101" s="12"/>
+      <c r="F101" s="12" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
@@ -2154,7 +2213,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
@@ -2164,17 +2223,21 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
-      <c r="D104" s="8"/>
+      <c r="D104" s="8">
+        <v>10</v>
+      </c>
       <c r="E104" s="8"/>
-      <c r="F104" s="12"/>
+      <c r="F104" s="12" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
-        <v>54</v>
+        <v>135</v>
       </c>
       <c r="B105" s="8"/>
       <c r="C105" s="8"/>
@@ -2184,7 +2247,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
-        <v>138</v>
+        <v>53</v>
       </c>
       <c r="B106" s="8"/>
       <c r="C106" s="8"/>
@@ -2194,7 +2257,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
@@ -2204,7 +2267,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B108" s="8"/>
       <c r="C108" s="8"/>
@@ -2214,17 +2277,19 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B109" s="8"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
-      <c r="E109" s="8"/>
+      <c r="E109" s="8" t="s">
+        <v>172</v>
+      </c>
       <c r="F109" s="12"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B110" s="8"/>
       <c r="C110" s="8"/>
@@ -2234,7 +2299,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="B111" s="8"/>
       <c r="C111" s="8"/>
@@ -2244,7 +2309,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="B112" s="8"/>
       <c r="C112" s="8"/>
@@ -2254,17 +2319,19 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="B113" s="8"/>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
       <c r="E113" s="8"/>
-      <c r="F113" s="12"/>
+      <c r="F113" s="12" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B114" s="8"/>
       <c r="C114" s="8"/>
@@ -2274,7 +2341,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B115" s="8"/>
       <c r="C115" s="8"/>
@@ -2284,7 +2351,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="11" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B116" s="8"/>
       <c r="C116" s="8"/>
@@ -2294,7 +2361,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="11" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B117" s="8"/>
       <c r="C117" s="8"/>
@@ -2304,7 +2371,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="11" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B118" s="8"/>
       <c r="C118" s="8"/>
@@ -2314,7 +2381,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="11" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B119" s="8"/>
       <c r="C119" s="8"/>
@@ -2324,7 +2391,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="11" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B120" s="8"/>
       <c r="C120" s="8"/>
@@ -2334,7 +2401,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="11" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
@@ -2344,7 +2411,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B122" s="8"/>
       <c r="C122" s="8"/>
@@ -2354,7 +2421,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="11" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B123" s="8"/>
       <c r="C123" s="8"/>
@@ -2364,7 +2431,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="11" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B124" s="8"/>
       <c r="C124" s="8"/>
@@ -2374,7 +2441,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B125" s="8"/>
       <c r="C125" s="8"/>
@@ -2384,7 +2451,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="11" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B126" s="8"/>
       <c r="C126" s="8"/>
@@ -2394,7 +2461,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="11" t="s">
-        <v>136</v>
+        <v>40</v>
       </c>
       <c r="B127" s="8"/>
       <c r="C127" s="8"/>
@@ -2404,7 +2471,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="11" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="B128" s="8"/>
       <c r="C128" s="8"/>
@@ -2414,7 +2481,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
@@ -2424,7 +2491,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="11" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
@@ -2434,7 +2501,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B131" s="8"/>
       <c r="C131" s="8"/>
@@ -2444,7 +2511,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="11" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B132" s="8"/>
       <c r="C132" s="8"/>
@@ -2454,7 +2521,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="11" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B133" s="8"/>
       <c r="C133" s="8"/>
@@ -2464,7 +2531,7 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="11" t="s">
-        <v>60</v>
+        <v>134</v>
       </c>
       <c r="B134" s="8"/>
       <c r="C134" s="8"/>
@@ -2474,7 +2541,7 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="B135" s="8"/>
       <c r="C135" s="8"/>
@@ -2484,7 +2551,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B136" s="8"/>
       <c r="C136" s="8"/>
@@ -2494,19 +2561,17 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B137" s="8"/>
       <c r="C137" s="8"/>
-      <c r="D137" s="8">
-        <v>10</v>
-      </c>
+      <c r="D137" s="8"/>
       <c r="E137" s="8"/>
       <c r="F137" s="12"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="11" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B138" s="8"/>
       <c r="C138" s="8"/>
@@ -2516,7 +2581,7 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B139" s="8"/>
       <c r="C139" s="8"/>
@@ -2526,7 +2591,7 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="11" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
@@ -2536,7 +2601,7 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="11" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
@@ -2545,101 +2610,173 @@
       <c r="F141" s="12"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" s="2"/>
-      <c r="B142" s="1"/>
-      <c r="C142" s="1"/>
-      <c r="D142" s="1"/>
-      <c r="E142" s="1"/>
-      <c r="F142" s="3"/>
+      <c r="A142" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B142" s="8"/>
+      <c r="C142" s="8"/>
+      <c r="D142" s="8"/>
+      <c r="E142" s="8"/>
+      <c r="F142" s="12"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B143" s="8"/>
+      <c r="C143" s="8"/>
+      <c r="D143" s="8"/>
+      <c r="E143" s="8"/>
+      <c r="F143" s="12"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B144" s="6"/>
-      <c r="C144" s="6"/>
-      <c r="D144" s="6"/>
-      <c r="E144" s="6"/>
-      <c r="F144" s="6"/>
+      <c r="A144" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B144" s="8"/>
+      <c r="C144" s="8"/>
+      <c r="D144" s="8">
+        <v>10</v>
+      </c>
+      <c r="E144" s="8"/>
+      <c r="F144" s="12"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B145" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C145" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D145" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E145" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F145" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="A145" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B145" s="8"/>
+      <c r="C145" s="8"/>
+      <c r="D145" s="8"/>
+      <c r="E145" s="8"/>
+      <c r="F145" s="12"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="8" t="s">
-        <v>121</v>
+      <c r="A146" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="B146" s="8"/>
       <c r="C146" s="8"/>
-      <c r="D146" s="8">
-        <v>10</v>
-      </c>
+      <c r="D146" s="8"/>
       <c r="E146" s="8"/>
-      <c r="F146" s="8"/>
-    </row>
-    <row r="147" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A147" s="8" t="s">
-        <v>130</v>
+      <c r="F146" s="12"/>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="B147" s="8"/>
       <c r="C147" s="8"/>
       <c r="D147" s="8"/>
       <c r="E147" s="8"/>
-      <c r="F147" s="9" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A148" s="8" t="s">
-        <v>156</v>
+      <c r="F147" s="12"/>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="B148" s="8"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
       <c r="E148" s="8"/>
-      <c r="F148" s="9" t="s">
-        <v>155</v>
-      </c>
+      <c r="F148" s="12"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="8" t="s">
+      <c r="A149" s="2"/>
+      <c r="B149" s="1"/>
+      <c r="C149" s="1"/>
+      <c r="D149" s="1"/>
+      <c r="E149" s="1"/>
+      <c r="F149" s="3"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B151" s="6"/>
+      <c r="C151" s="6"/>
+      <c r="D151" s="6"/>
+      <c r="E151" s="6"/>
+      <c r="F151" s="6"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C152" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D152" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E152" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F152" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B153" s="8"/>
+      <c r="C153" s="8"/>
+      <c r="D153" s="8">
+        <v>10</v>
+      </c>
+      <c r="E153" s="8"/>
+      <c r="F153" s="8"/>
+    </row>
+    <row r="154" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A154" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B154" s="8"/>
+      <c r="C154" s="8"/>
+      <c r="D154" s="8"/>
+      <c r="E154" s="8"/>
+      <c r="F154" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A155" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B155" s="8"/>
+      <c r="C155" s="8"/>
+      <c r="D155" s="8"/>
+      <c r="E155" s="8"/>
+      <c r="F155" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B149" s="8"/>
-      <c r="C149" s="8"/>
-      <c r="D149" s="8"/>
-      <c r="E149" s="8"/>
-      <c r="F149" s="9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B150" s="8"/>
-      <c r="C150" s="8"/>
-      <c r="D150" s="8"/>
-      <c r="E150" s="8"/>
-      <c r="F150" s="9" t="s">
-        <v>154</v>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B156" s="8"/>
+      <c r="C156" s="8"/>
+      <c r="D156" s="8"/>
+      <c r="E156" s="8"/>
+      <c r="F156" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A157" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B157" s="8"/>
+      <c r="C157" s="8"/>
+      <c r="D157" s="8"/>
+      <c r="E157" s="8"/>
+      <c r="F157" s="9" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>